<commit_message>
Finalize plots of weights
</commit_message>
<xml_diff>
--- a/analysis/derived_data/ISEA_use-wear_weights.xlsx
+++ b/analysis/derived_data/ISEA_use-wear_weights.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,15 +360,25 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Tool</t>
+          <t>Sample</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Chert_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Chert_tool</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Weight_before_[mg]</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Weight_after_[mg]</t>
         </is>
@@ -377,156 +387,252 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A1</t>
-        </is>
-      </c>
-      <c r="B2">
+          <t>ISEA-EX1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>30.07</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B1</t>
-        </is>
-      </c>
-      <c r="B3">
+          <t>ISEA-EX2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>21.52</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>21.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A2</t>
-        </is>
-      </c>
-      <c r="B4">
+          <t>ISEA-EX3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>28.65</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>28.62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B2</t>
-        </is>
-      </c>
-      <c r="B5">
+          <t>ISEA-EX4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>16.69</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>16.67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A3</t>
-        </is>
-      </c>
-      <c r="B6">
+          <t>ISEA-EX5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
         <v>16.69</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>16.66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B3</t>
-        </is>
-      </c>
-      <c r="B7">
+          <t>ISEA-EX6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>10.25</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>10.04</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A4</t>
-        </is>
-      </c>
-      <c r="B8">
+          <t>ISEA-EX7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>18.25</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>18.24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B4</t>
-        </is>
-      </c>
-      <c r="B9">
+          <t>ISEA-EX8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
         <v>13.49</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>13.48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A5</t>
-        </is>
-      </c>
-      <c r="B10">
+          <t>ISEA-EX9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
         <v>24.6</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>24.44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B5</t>
-        </is>
-      </c>
-      <c r="B11">
+          <t>ISEA-EX10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
         <v>17.04</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ISEA-Chert-A6</t>
-        </is>
-      </c>
-      <c r="B12">
+          <t>ISEA-EX11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
         <v>15.32</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>15.31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ISEA-Chert-B6</t>
-        </is>
-      </c>
-      <c r="B13">
+          <t>ISEA-EX12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
         <v>16.76</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>16.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Bamboo species for plots and summary stats
</commit_message>
<xml_diff>
--- a/analysis/derived_data/ISEA_use-wear_weights.xlsx
+++ b/analysis/derived_data/ISEA_use-wear_weights.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,10 +375,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Bamboo_sp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Weight_before_[mg]</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Weight_after_[mg]</t>
         </is>
@@ -398,10 +403,15 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E2">
         <v>30.07</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>30</v>
       </c>
     </row>
@@ -419,10 +429,15 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E3">
         <v>21.52</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>21.5</v>
       </c>
     </row>
@@ -440,10 +455,15 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E4">
         <v>28.65</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>28.62</v>
       </c>
     </row>
@@ -461,10 +481,15 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E5">
         <v>16.69</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>16.67</v>
       </c>
     </row>
@@ -482,10 +507,15 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E6">
         <v>16.69</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>16.66</v>
       </c>
     </row>
@@ -503,10 +533,15 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="E7">
         <v>10.25</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>10.04</v>
       </c>
     </row>
@@ -524,10 +559,15 @@
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E8">
         <v>18.25</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>18.24</v>
       </c>
     </row>
@@ -545,10 +585,15 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E9">
         <v>13.49</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>13.48</v>
       </c>
     </row>
@@ -566,10 +611,15 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E10">
         <v>24.6</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>24.44</v>
       </c>
     </row>
@@ -587,10 +637,15 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E11">
         <v>17.04</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>17</v>
       </c>
     </row>
@@ -608,10 +663,15 @@
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E12">
         <v>15.32</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>15.31</v>
       </c>
     </row>
@@ -629,10 +689,15 @@
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="E13">
         <v>16.76</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>16.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed: names of Chert_type in weight dataset
</commit_message>
<xml_diff>
--- a/analysis/derived_data/ISEA_use-wear_weights.xlsx
+++ b/analysis/derived_data/ISEA_use-wear_weights.xlsx
@@ -397,7 +397,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C2">
@@ -423,7 +423,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C3">
@@ -449,7 +449,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C4">
@@ -475,7 +475,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C5">
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C6">
@@ -527,7 +527,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C7">
@@ -553,7 +553,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C8">
@@ -579,7 +579,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C9">
@@ -605,7 +605,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C10">
@@ -631,7 +631,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C11">
@@ -657,7 +657,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C12">
@@ -683,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C13">

</xml_diff>